<commit_message>
add a slot in AssignTable for NEXT_WEEK to eliminate judgment in isValidPrior(). make the code available to compiled with g++. log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/compare--20150501--GreedyInit+Tabu.xlsx
+++ b/INRC2_Simulator/log/compare--20150501--GreedyInit+Tabu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16830" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="18000" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
-  <si>
-    <t>1;1.2,1.2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
   <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -93,6 +89,10 @@
   </si>
   <si>
     <t>1;1.2,1.2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;1.2,1.2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -755,14 +755,14 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -809,119 +809,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -1261,9 +1149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1280,87 +1166,87 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7"/>
+      <c r="F2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1413,10 +1299,10 @@
       <c r="A5" s="5">
         <v>415</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>415</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>415</v>
       </c>
       <c r="D5" s="5">
@@ -1428,19 +1314,19 @@
       <c r="F5" s="4">
         <v>415</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>415</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>415</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>415</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <v>415</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>415</v>
       </c>
     </row>
@@ -1448,10 +1334,10 @@
       <c r="A6" s="5">
         <v>450.83300000000003</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>473.33300000000003</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>459.16699999999997</v>
       </c>
       <c r="D6" s="5">
@@ -1463,19 +1349,19 @@
       <c r="F6" s="4">
         <v>465.83300000000003</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>451.66699999999997</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>466.66699999999997</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>445.83300000000003</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>445.83300000000003</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <v>459.16699999999997</v>
       </c>
     </row>
@@ -1483,10 +1369,10 @@
       <c r="A7" s="5">
         <v>442.5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>435.83300000000003</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>425.83300000000003</v>
       </c>
       <c r="D7" s="5">
@@ -1498,19 +1384,19 @@
       <c r="F7" s="4">
         <v>442.5</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>434.16699999999997</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>425.83300000000003</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>418.33300000000003</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>438.33300000000003</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>427.5</v>
       </c>
     </row>
@@ -1518,10 +1404,10 @@
       <c r="A8" s="5">
         <v>348.33300000000003</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>375</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>332.5</v>
       </c>
       <c r="D8" s="5">
@@ -1533,19 +1419,19 @@
       <c r="F8" s="4">
         <v>352.5</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>355.83300000000003</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>350</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>330</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <v>355.83300000000003</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>356.66699999999997</v>
       </c>
     </row>
@@ -1553,10 +1439,10 @@
       <c r="A9" s="5">
         <v>337.5</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>337.5</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>337.5</v>
       </c>
       <c r="D9" s="5">
@@ -1568,19 +1454,19 @@
       <c r="F9" s="4">
         <v>337.5</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>337.5</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>337.5</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>337.70800000000003</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <v>337.5</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>337.5</v>
       </c>
     </row>
@@ -1588,10 +1474,10 @@
       <c r="A10" s="5">
         <v>322.91699999999997</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>328.33300000000003</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>320.83300000000003</v>
       </c>
       <c r="D10" s="5">
@@ -1603,19 +1489,19 @@
       <c r="F10" s="4">
         <v>319.58300000000003</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>321.66699999999997</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>315.41699999999997</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>316.45800000000003</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <v>316.66699999999997</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <v>326.66699999999997</v>
       </c>
     </row>
@@ -1623,10 +1509,10 @@
       <c r="A11" s="5">
         <v>526.04200000000003</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>507.5</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>486.25</v>
       </c>
       <c r="D11" s="5">
@@ -1638,19 +1524,19 @@
       <c r="F11" s="4">
         <v>521.04200000000003</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>508.75</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>492.29199999999997</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>511.66699999999997</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <v>497.91699999999997</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="7">
         <v>517.08299999999997</v>
       </c>
     </row>
@@ -1658,10 +1544,10 @@
       <c r="A12" s="5">
         <v>318.54199999999997</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>312.5</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>313.75</v>
       </c>
       <c r="D12" s="5">
@@ -1673,19 +1559,19 @@
       <c r="F12" s="4">
         <v>338.54199999999997</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>324.58300000000003</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>318.95800000000003</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>326.66699999999997</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <v>302.91699999999997</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <v>330.41699999999997</v>
       </c>
     </row>
@@ -1693,10 +1579,10 @@
       <c r="A13" s="5">
         <v>359.58300000000003</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>346.25</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>359.58300000000003</v>
       </c>
       <c r="D13" s="5">
@@ -1708,19 +1594,19 @@
       <c r="F13" s="4">
         <v>380.41699999999997</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>363.75</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>347.5</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>359.58300000000003</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>361.25</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>358.33300000000003</v>
       </c>
     </row>
@@ -1728,10 +1614,10 @@
       <c r="A14" s="5">
         <v>470</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>467.08300000000003</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>458.75</v>
       </c>
       <c r="D14" s="5">
@@ -1743,19 +1629,19 @@
       <c r="F14" s="4">
         <v>443.75</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>474.58300000000003</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>459.58300000000003</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>472.08300000000003</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="7">
         <v>457.5</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <v>454.16699999999997</v>
       </c>
     </row>
@@ -1763,10 +1649,10 @@
       <c r="A15" s="5">
         <v>492.91699999999997</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>498.33300000000003</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>519.58299999999997</v>
       </c>
       <c r="D15" s="5">
@@ -1778,19 +1664,19 @@
       <c r="F15" s="4">
         <v>498.33300000000003</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>498.33300000000003</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <v>505.83300000000003</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>501.66699999999997</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <v>509.58300000000003</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="7">
         <v>497.91699999999997</v>
       </c>
     </row>
@@ -1798,10 +1684,10 @@
       <c r="A16" s="5">
         <v>380</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>411.66699999999997</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>393.75</v>
       </c>
       <c r="D16" s="5">
@@ -1813,19 +1699,19 @@
       <c r="F16" s="4">
         <v>394.16699999999997</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <v>403.33300000000003</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>391.25</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>394.16699999999997</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="7">
         <v>392.5</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="7">
         <v>409.58300000000003</v>
       </c>
     </row>
@@ -1833,10 +1719,10 @@
       <c r="A17" s="5">
         <v>560</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>570</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>570</v>
       </c>
       <c r="D17" s="5">
@@ -1848,19 +1734,19 @@
       <c r="F17" s="4">
         <v>582.08299999999997</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <v>573.75</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <v>561.66700000000003</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>567.91700000000003</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="7">
         <v>565.83299999999997</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="7">
         <v>561.66700000000003</v>
       </c>
     </row>
@@ -1868,10 +1754,10 @@
       <c r="A18" s="5">
         <v>569.16700000000003</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>580.83299999999997</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>592.5</v>
       </c>
       <c r="D18" s="5">
@@ -1883,19 +1769,19 @@
       <c r="F18" s="4">
         <v>591.25</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>588.75</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="7">
         <v>577.5</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>585.41700000000003</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="7">
         <v>591.66700000000003</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="7">
         <v>582.5</v>
       </c>
     </row>
@@ -1903,10 +1789,10 @@
       <c r="A19" s="5">
         <v>447.08300000000003</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>470.41699999999997</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>469.16699999999997</v>
       </c>
       <c r="D19" s="5">
@@ -1918,19 +1804,19 @@
       <c r="F19" s="4">
         <v>452.5</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>490.41699999999997</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="7">
         <v>467.91699999999997</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="7">
         <v>477.5</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="7">
         <v>464.58300000000003</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="7">
         <v>462.91699999999997</v>
       </c>
     </row>
@@ -1938,10 +1824,10 @@
       <c r="A20" s="5">
         <v>458.75</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>437.91699999999997</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>449.16699999999997</v>
       </c>
       <c r="D20" s="5">
@@ -1953,19 +1839,19 @@
       <c r="F20" s="4">
         <v>443.33300000000003</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>429.58300000000003</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <v>464.58300000000003</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>441.66699999999997</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="7">
         <v>457.08300000000003</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="7">
         <v>434.58300000000003</v>
       </c>
     </row>
@@ -1973,10 +1859,10 @@
       <c r="A21" s="5">
         <v>740.41700000000003</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>747.08299999999997</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>742.08299999999997</v>
       </c>
       <c r="D21" s="5">
@@ -1988,19 +1874,19 @@
       <c r="F21" s="4">
         <v>752.08299999999997</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>744.16700000000003</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="7">
         <v>735.83299999999997</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <v>742.5</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="7">
         <v>738.33299999999997</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="7">
         <v>735.83299999999997</v>
       </c>
     </row>
@@ -2008,10 +1894,10 @@
       <c r="A22" s="5">
         <v>635.41700000000003</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <v>651.25</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>667.08299999999997</v>
       </c>
       <c r="D22" s="5">
@@ -2023,19 +1909,19 @@
       <c r="F22" s="4">
         <v>665.41700000000003</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <v>647.5</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="7">
         <v>641.66700000000003</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="7">
         <v>640.83299999999997</v>
       </c>
-      <c r="J22" s="8">
+      <c r="J22" s="7">
         <v>645</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22" s="7">
         <v>659.16700000000003</v>
       </c>
     </row>
@@ -2043,10 +1929,10 @@
       <c r="A23" s="5">
         <v>399.58300000000003</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="7">
         <v>395.41699999999997</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>405.41699999999997</v>
       </c>
       <c r="D23" s="5">
@@ -2058,19 +1944,19 @@
       <c r="F23" s="4">
         <v>426.25</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="8">
         <v>412.5</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>400.41699999999997</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="7">
         <v>405.41699999999997</v>
       </c>
-      <c r="J23" s="8">
+      <c r="J23" s="7">
         <v>402.5</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K23" s="7">
         <v>410</v>
       </c>
     </row>
@@ -2078,10 +1964,10 @@
       <c r="A24" s="5">
         <v>563.75</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="7">
         <v>577.91700000000003</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>586.25</v>
       </c>
       <c r="D24" s="5">
@@ -2093,19 +1979,19 @@
       <c r="F24" s="4">
         <v>605.41700000000003</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <v>601.66700000000003</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="7">
         <v>595.41700000000003</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="7">
         <v>612.08299999999997</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="7">
         <v>593.33299999999997</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="7">
         <v>602.5</v>
       </c>
     </row>
@@ -2113,10 +1999,10 @@
       <c r="A25" s="5">
         <v>514.16700000000003</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="7">
         <v>529.58299999999997</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>545.41700000000003</v>
       </c>
       <c r="D25" s="5">
@@ -2128,19 +2014,19 @@
       <c r="F25" s="4">
         <v>557.08299999999997</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="8">
         <v>533.33299999999997</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="7">
         <v>524.16700000000003</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="7">
         <v>526.66700000000003</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="7">
         <v>521.25</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="7">
         <v>519.58299999999997</v>
       </c>
     </row>
@@ -2148,10 +2034,10 @@
       <c r="A26" s="5">
         <v>295.83300000000003</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="7">
         <v>316.25</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>316.25</v>
       </c>
       <c r="D26" s="5">
@@ -2163,19 +2049,19 @@
       <c r="F26" s="4">
         <v>319.58300000000003</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <v>314.16699999999997</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="7">
         <v>310.83300000000003</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="7">
         <v>303.33300000000003</v>
       </c>
-      <c r="J26" s="8">
+      <c r="J26" s="7">
         <v>292.91699999999997</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="7">
         <v>308.75</v>
       </c>
     </row>
@@ -2183,10 +2069,10 @@
       <c r="A27" s="5">
         <v>481.25</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="7">
         <v>517.91700000000003</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>495</v>
       </c>
       <c r="D27" s="5">
@@ -2198,19 +2084,19 @@
       <c r="F27" s="4">
         <v>507.91699999999997</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="8">
         <v>503.33300000000003</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="7">
         <v>492.08300000000003</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="7">
         <v>491.66699999999997</v>
       </c>
-      <c r="J27" s="8">
+      <c r="J27" s="7">
         <v>493.33300000000003</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="7">
         <v>496.25</v>
       </c>
     </row>
@@ -2218,10 +2104,10 @@
       <c r="A28" s="5">
         <v>431.25</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="7">
         <v>416.25</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>420.83300000000003</v>
       </c>
       <c r="D28" s="5">
@@ -2233,19 +2119,19 @@
       <c r="F28" s="4">
         <v>431.25</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="8">
         <v>439.16699999999997</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="7">
         <v>427.91699999999997</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="7">
         <v>417.5</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J28" s="7">
         <v>432.5</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28" s="7">
         <v>431.25</v>
       </c>
     </row>
@@ -2253,10 +2139,10 @@
       <c r="A29" s="5">
         <v>378.33300000000003</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="7">
         <v>346.25</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>363.33300000000003</v>
       </c>
       <c r="D29" s="5">
@@ -2268,19 +2154,19 @@
       <c r="F29" s="4">
         <v>372.08300000000003</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="8">
         <v>369.16699999999997</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="7">
         <v>375</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="7">
         <v>355</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="7">
         <v>368.75</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="7">
         <v>351.25</v>
       </c>
     </row>
@@ -2288,10 +2174,10 @@
       <c r="A30" s="5">
         <v>538.33299999999997</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>509.58300000000003</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>485</v>
       </c>
       <c r="D30" s="5">
@@ -2303,19 +2189,19 @@
       <c r="F30" s="4">
         <v>525.41700000000003</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="8">
         <v>507.5</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="7">
         <v>511.66699999999997</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="7">
         <v>510.83300000000003</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J30" s="7">
         <v>541.25</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30" s="7">
         <v>502.91699999999997</v>
       </c>
     </row>
@@ -2323,10 +2209,10 @@
       <c r="A31" s="5">
         <v>481.66699999999997</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="7">
         <v>430</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>431.66699999999997</v>
       </c>
       <c r="D31" s="5">
@@ -2338,19 +2224,19 @@
       <c r="F31" s="4">
         <v>457.5</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="8">
         <v>452.91699999999997</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="7">
         <v>477.91699999999997</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I31" s="7">
         <v>485</v>
       </c>
-      <c r="J31" s="8">
+      <c r="J31" s="7">
         <v>491.66699999999997</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31" s="7">
         <v>462.5</v>
       </c>
     </row>
@@ -2358,10 +2244,10 @@
       <c r="A32" s="5">
         <v>315</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7">
         <v>285</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <v>311.66699999999997</v>
       </c>
       <c r="D32" s="5">
@@ -2373,19 +2259,19 @@
       <c r="F32" s="4">
         <v>311.66699999999997</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="8">
         <v>330.41699999999997</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="7">
         <v>317.08300000000003</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="7">
         <v>345.83300000000003</v>
       </c>
-      <c r="J32" s="8">
+      <c r="J32" s="7">
         <v>326.66699999999997</v>
       </c>
-      <c r="K32" s="8">
+      <c r="K32" s="7">
         <v>321.66699999999997</v>
       </c>
     </row>
@@ -2393,10 +2279,10 @@
       <c r="A33" s="5">
         <v>623.33299999999997</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="7">
         <v>647.91700000000003</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>644.16700000000003</v>
       </c>
       <c r="D33" s="5">
@@ -2408,19 +2294,19 @@
       <c r="F33" s="4">
         <v>660</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="8">
         <v>639.58299999999997</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="7">
         <v>620</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="7">
         <v>636.66700000000003</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J33" s="7">
         <v>633.75</v>
       </c>
-      <c r="K33" s="8">
+      <c r="K33" s="7">
         <v>627.91700000000003</v>
       </c>
     </row>
@@ -2428,10 +2314,10 @@
       <c r="A34" s="5">
         <v>507.5</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="7">
         <v>535.41700000000003</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>533.33299999999997</v>
       </c>
       <c r="D34" s="5">
@@ -2443,19 +2329,19 @@
       <c r="F34" s="4">
         <v>566.66700000000003</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="8">
         <v>527.08299999999997</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="7">
         <v>517.5</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="7">
         <v>495</v>
       </c>
-      <c r="J34" s="8">
+      <c r="J34" s="7">
         <v>517.91700000000003</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34" s="7">
         <v>520.41700000000003</v>
       </c>
     </row>
@@ -2463,10 +2349,10 @@
       <c r="A35" s="5">
         <v>593.33299999999997</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="7">
         <v>627.08299999999997</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>598.75</v>
       </c>
       <c r="D35" s="5">
@@ -2478,19 +2364,19 @@
       <c r="F35" s="4">
         <v>623.75</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="8">
         <v>617.5</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="7">
         <v>603.33299999999997</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="7">
         <v>597.5</v>
       </c>
-      <c r="J35" s="8">
+      <c r="J35" s="7">
         <v>611.25</v>
       </c>
-      <c r="K35" s="8">
+      <c r="K35" s="7">
         <v>627.08299999999997</v>
       </c>
     </row>
@@ -2498,10 +2384,10 @@
       <c r="A36" s="5">
         <v>468.33300000000003</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="7">
         <v>484.58300000000003</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <v>486.25</v>
       </c>
       <c r="D36" s="5">
@@ -2513,19 +2399,19 @@
       <c r="F36" s="4">
         <v>475.41699999999997</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="8">
         <v>500</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="7">
         <v>487.5</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="7">
         <v>452.5</v>
       </c>
-      <c r="J36" s="8">
+      <c r="J36" s="7">
         <v>471.25</v>
       </c>
-      <c r="K36" s="8">
+      <c r="K36" s="7">
         <v>489.58300000000003</v>
       </c>
     </row>
@@ -2533,10 +2419,10 @@
       <c r="A37" s="5">
         <v>600.41700000000003</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="7">
         <v>620</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>634.16700000000003</v>
       </c>
       <c r="D37" s="5">
@@ -2548,19 +2434,19 @@
       <c r="F37" s="4">
         <v>626.25</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="8">
         <v>636.45799999999997</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="7">
         <v>606.45799999999997</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="7">
         <v>602.5</v>
       </c>
-      <c r="J37" s="8">
+      <c r="J37" s="7">
         <v>602.08299999999997</v>
       </c>
-      <c r="K37" s="8">
+      <c r="K37" s="7">
         <v>602.70799999999997</v>
       </c>
     </row>
@@ -2568,10 +2454,10 @@
       <c r="A38" s="5">
         <v>527.08299999999997</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7">
         <v>557.5</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <v>545</v>
       </c>
       <c r="D38" s="5">
@@ -2583,19 +2469,19 @@
       <c r="F38" s="4">
         <v>549.16700000000003</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="8">
         <v>551.04200000000003</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="7">
         <v>530.625</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="7">
         <v>523.75</v>
       </c>
-      <c r="J38" s="8">
+      <c r="J38" s="7">
         <v>517.5</v>
       </c>
-      <c r="K38" s="8">
+      <c r="K38" s="7">
         <v>523.125</v>
       </c>
     </row>
@@ -2603,10 +2489,10 @@
       <c r="A39" s="5">
         <v>423.75</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="7">
         <v>443.54199999999997</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="7">
         <v>436.25</v>
       </c>
       <c r="D39" s="5">
@@ -2618,19 +2504,19 @@
       <c r="F39" s="4">
         <v>453.95800000000003</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="8">
         <v>428.95800000000003</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="7">
         <v>414.79199999999997</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="7">
         <v>426.45800000000003</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J39" s="7">
         <v>437.29199999999997</v>
       </c>
-      <c r="K39" s="8">
+      <c r="K39" s="7">
         <v>443.54199999999997</v>
       </c>
     </row>
@@ -2638,10 +2524,10 @@
       <c r="A40" s="5">
         <v>441.25</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="7">
         <v>451.45800000000003</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="7">
         <v>470.41699999999997</v>
       </c>
       <c r="D40" s="5">
@@ -2653,19 +2539,19 @@
       <c r="F40" s="4">
         <v>479.79199999999997</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="8">
         <v>448.54199999999997</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="7">
         <v>464.79199999999997</v>
       </c>
-      <c r="I40" s="8">
+      <c r="I40" s="7">
         <v>452.29199999999997</v>
       </c>
-      <c r="J40" s="8">
+      <c r="J40" s="7">
         <v>455.625</v>
       </c>
-      <c r="K40" s="8">
+      <c r="K40" s="7">
         <v>445.625</v>
       </c>
     </row>
@@ -2673,10 +2559,10 @@
       <c r="A41" s="5">
         <v>349.58300000000003</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="7">
         <v>385.20800000000003</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="7">
         <v>355.625</v>
       </c>
       <c r="D41" s="5">
@@ -2688,19 +2574,19 @@
       <c r="F41" s="4">
         <v>400.83300000000003</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="8">
         <v>382.29199999999997</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="7">
         <v>364.375</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="7">
         <v>372.70800000000003</v>
       </c>
-      <c r="J41" s="8">
+      <c r="J41" s="7">
         <v>385.20800000000003</v>
       </c>
-      <c r="K41" s="8">
+      <c r="K41" s="7">
         <v>360.20800000000003</v>
       </c>
     </row>
@@ -2708,10 +2594,10 @@
       <c r="A42" s="5">
         <v>412.08300000000003</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>431.45800000000003</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="7">
         <v>427.70800000000003</v>
       </c>
       <c r="D42" s="5">
@@ -2723,19 +2609,19 @@
       <c r="F42" s="4">
         <v>442.91699999999997</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="8">
         <v>453.125</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="7">
         <v>436.04199999999997</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I42" s="7">
         <v>413.125</v>
       </c>
-      <c r="J42" s="8">
+      <c r="J42" s="7">
         <v>426.04199999999997</v>
       </c>
-      <c r="K42" s="8">
+      <c r="K42" s="7">
         <v>440.625</v>
       </c>
     </row>
@@ -2743,10 +2629,10 @@
       <c r="A43" s="5">
         <v>427.91699999999997</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="7">
         <v>491.66699999999997</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="7">
         <v>486.04199999999997</v>
       </c>
       <c r="D43" s="5">
@@ -2758,19 +2644,19 @@
       <c r="F43" s="4">
         <v>472.5</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="8">
         <v>497.91699999999997</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="7">
         <v>512.29200000000003</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I43" s="7">
         <v>471.875</v>
       </c>
-      <c r="J43" s="8">
+      <c r="J43" s="7">
         <v>483.75</v>
       </c>
-      <c r="K43" s="8">
+      <c r="K43" s="7">
         <v>492.5</v>
       </c>
     </row>
@@ -2778,10 +2664,10 @@
       <c r="A44" s="5">
         <v>395.41699999999997</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7">
         <v>477.5</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="7">
         <v>434.79199999999997</v>
       </c>
       <c r="D44" s="5">
@@ -2793,19 +2679,19 @@
       <c r="F44" s="4">
         <v>518.75</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="8">
         <v>448.33300000000003</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H44" s="7">
         <v>408.95800000000003</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="7">
         <v>471.45800000000003</v>
       </c>
-      <c r="J44" s="8">
+      <c r="J44" s="7">
         <v>452.5</v>
       </c>
-      <c r="K44" s="8">
+      <c r="K44" s="7">
         <v>460</v>
       </c>
     </row>
@@ -2813,10 +2699,10 @@
       <c r="A45" s="5">
         <v>923.33299999999997</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>962.91700000000003</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="7">
         <v>954.58299999999997</v>
       </c>
       <c r="D45" s="5">
@@ -2828,19 +2714,19 @@
       <c r="F45" s="4">
         <v>986.66700000000003</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="8">
         <v>943.33299999999997</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45" s="7">
         <v>927.5</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="7">
         <v>925.41700000000003</v>
       </c>
-      <c r="J45" s="8">
+      <c r="J45" s="7">
         <v>929.16700000000003</v>
       </c>
-      <c r="K45" s="8">
+      <c r="K45" s="7">
         <v>927.5</v>
       </c>
     </row>
@@ -2848,10 +2734,10 @@
       <c r="A46" s="5">
         <v>445</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="7">
         <v>472.91699999999997</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="7">
         <v>515.41700000000003</v>
       </c>
       <c r="D46" s="5">
@@ -2863,19 +2749,19 @@
       <c r="F46" s="4">
         <v>525.83299999999997</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="8">
         <v>471.66699999999997</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="7">
         <v>473.33300000000003</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="7">
         <v>455.41699999999997</v>
       </c>
-      <c r="J46" s="8">
+      <c r="J46" s="7">
         <v>445</v>
       </c>
-      <c r="K46" s="8">
+      <c r="K46" s="7">
         <v>437.5</v>
       </c>
     </row>
@@ -2883,10 +2769,10 @@
       <c r="A47" s="5">
         <v>652.5</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>630.83299999999997</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="7">
         <v>660.83299999999997</v>
       </c>
       <c r="D47" s="5">
@@ -2898,19 +2784,19 @@
       <c r="F47" s="4">
         <v>653.75</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="8">
         <v>646.66700000000003</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="7">
         <v>666.25</v>
       </c>
-      <c r="I47" s="8">
+      <c r="I47" s="7">
         <v>664.16700000000003</v>
       </c>
-      <c r="J47" s="8">
+      <c r="J47" s="7">
         <v>672.08299999999997</v>
       </c>
-      <c r="K47" s="8">
+      <c r="K47" s="7">
         <v>664.16700000000003</v>
       </c>
     </row>
@@ -2918,10 +2804,10 @@
       <c r="A48" s="5">
         <v>340.83300000000003</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="7">
         <v>354.16699999999997</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="7">
         <v>348.33300000000003</v>
       </c>
       <c r="D48" s="5">
@@ -2933,19 +2819,19 @@
       <c r="F48" s="4">
         <v>330.41699999999997</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="8">
         <v>320.83300000000003</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="7">
         <v>349.58300000000003</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="7">
         <v>355</v>
       </c>
-      <c r="J48" s="8">
+      <c r="J48" s="7">
         <v>349.58300000000003</v>
       </c>
-      <c r="K48" s="8">
+      <c r="K48" s="7">
         <v>333.33300000000003</v>
       </c>
     </row>
@@ -2953,10 +2839,10 @@
       <c r="A49" s="5">
         <v>994.16700000000003</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>1045</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="7">
         <v>1040.83</v>
       </c>
       <c r="D49" s="5">
@@ -2968,19 +2854,19 @@
       <c r="F49" s="4">
         <v>1060.83</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="8">
         <v>1037.5</v>
       </c>
-      <c r="H49" s="8">
+      <c r="H49" s="7">
         <v>1011.67</v>
       </c>
-      <c r="I49" s="8">
+      <c r="I49" s="7">
         <v>1005</v>
       </c>
-      <c r="J49" s="8">
+      <c r="J49" s="7">
         <v>998.33299999999997</v>
       </c>
-      <c r="K49" s="8">
+      <c r="K49" s="7">
         <v>1013.33</v>
       </c>
     </row>
@@ -2988,10 +2874,10 @@
       <c r="A50" s="5">
         <v>816.66700000000003</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" s="7">
         <v>855.83299999999997</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="7">
         <v>835.83299999999997</v>
       </c>
       <c r="D50" s="5">
@@ -3003,19 +2889,19 @@
       <c r="F50" s="4">
         <v>844.16700000000003</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="8">
         <v>877.5</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H50" s="7">
         <v>835</v>
       </c>
-      <c r="I50" s="8">
+      <c r="I50" s="7">
         <v>830</v>
       </c>
-      <c r="J50" s="8">
+      <c r="J50" s="7">
         <v>815</v>
       </c>
-      <c r="K50" s="8">
+      <c r="K50" s="7">
         <v>824.16700000000003</v>
       </c>
     </row>
@@ -3023,10 +2909,10 @@
       <c r="A51" s="5">
         <v>897.5</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="7">
         <v>935</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="7">
         <v>944.58299999999997</v>
       </c>
       <c r="D51" s="5">
@@ -3038,19 +2924,19 @@
       <c r="F51" s="4">
         <v>964.58299999999997</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="8">
         <v>942.5</v>
       </c>
-      <c r="H51" s="8">
+      <c r="H51" s="7">
         <v>919.58299999999997</v>
       </c>
-      <c r="I51" s="8">
+      <c r="I51" s="7">
         <v>946.66700000000003</v>
       </c>
-      <c r="J51" s="8">
+      <c r="J51" s="7">
         <v>913.33299999999997</v>
       </c>
-      <c r="K51" s="8">
+      <c r="K51" s="7">
         <v>910.41700000000003</v>
       </c>
     </row>
@@ -3058,10 +2944,10 @@
       <c r="A52" s="5">
         <v>1005.83</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="7">
         <v>968.33299999999997</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="7">
         <v>1022.08</v>
       </c>
       <c r="D52" s="5">
@@ -3073,19 +2959,19 @@
       <c r="F52" s="4">
         <v>994.58299999999997</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="8">
         <v>980.83299999999997</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H52" s="7">
         <v>1028.75</v>
       </c>
-      <c r="I52" s="8">
+      <c r="I52" s="7">
         <v>1058.33</v>
       </c>
-      <c r="J52" s="8">
+      <c r="J52" s="7">
         <v>1044.17</v>
       </c>
-      <c r="K52" s="8">
+      <c r="K52" s="7">
         <v>1007.92</v>
       </c>
     </row>
@@ -3093,10 +2979,10 @@
       <c r="A53" s="5">
         <v>791.66700000000003</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="7">
         <v>787.08299999999997</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="7">
         <v>768.33299999999997</v>
       </c>
       <c r="D53" s="5">
@@ -3108,19 +2994,19 @@
       <c r="F53" s="4">
         <v>764.16700000000003</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="8">
         <v>827.91700000000003</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="7">
         <v>765.83299999999997</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="7">
         <v>808.33299999999997</v>
       </c>
-      <c r="J53" s="8">
+      <c r="J53" s="7">
         <v>816.66700000000003</v>
       </c>
-      <c r="K53" s="8">
+      <c r="K53" s="7">
         <v>780</v>
       </c>
     </row>
@@ -3128,10 +3014,10 @@
       <c r="A54" s="5">
         <v>832.5</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="7">
         <v>829.58299999999997</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="7">
         <v>852.5</v>
       </c>
       <c r="D54" s="5">
@@ -3143,19 +3029,19 @@
       <c r="F54" s="4">
         <v>851.66700000000003</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="8">
         <v>872.91700000000003</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="7">
         <v>837.5</v>
       </c>
-      <c r="I54" s="8">
+      <c r="I54" s="7">
         <v>833.33299999999997</v>
       </c>
-      <c r="J54" s="8">
+      <c r="J54" s="7">
         <v>866.66700000000003</v>
       </c>
-      <c r="K54" s="8">
+      <c r="K54" s="7">
         <v>874.16700000000003</v>
       </c>
     </row>
@@ -3163,10 +3049,10 @@
       <c r="A55" s="5">
         <v>928.33299999999997</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="7">
         <v>892.5</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="7">
         <v>896.25</v>
       </c>
       <c r="D55" s="5">
@@ -3178,19 +3064,19 @@
       <c r="F55" s="4">
         <v>865.83299999999997</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="8">
         <v>914.16700000000003</v>
       </c>
-      <c r="H55" s="8">
+      <c r="H55" s="7">
         <v>884.58299999999997</v>
       </c>
-      <c r="I55" s="8">
+      <c r="I55" s="7">
         <v>932.5</v>
       </c>
-      <c r="J55" s="8">
+      <c r="J55" s="7">
         <v>854.16700000000003</v>
       </c>
-      <c r="K55" s="8">
+      <c r="K55" s="7">
         <v>851.25</v>
       </c>
     </row>
@@ -3198,10 +3084,10 @@
       <c r="A56" s="5">
         <v>929.16700000000003</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56" s="7">
         <v>871.66700000000003</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="7">
         <v>849.58299999999997</v>
       </c>
       <c r="D56" s="5">
@@ -3213,19 +3099,19 @@
       <c r="F56" s="4">
         <v>876.66700000000003</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="8">
         <v>937.5</v>
       </c>
-      <c r="H56" s="8">
+      <c r="H56" s="7">
         <v>919.58299999999997</v>
       </c>
-      <c r="I56" s="8">
+      <c r="I56" s="7">
         <v>931.66700000000003</v>
       </c>
-      <c r="J56" s="8">
+      <c r="J56" s="7">
         <v>925.83299999999997</v>
       </c>
-      <c r="K56" s="8">
+      <c r="K56" s="7">
         <v>888.75</v>
       </c>
     </row>
@@ -3233,10 +3119,10 @@
       <c r="A57" s="5">
         <v>1088.75</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57" s="7">
         <v>1121.67</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C57" s="7">
         <v>1119.17</v>
       </c>
       <c r="D57" s="5">
@@ -3248,19 +3134,19 @@
       <c r="F57" s="4">
         <v>1164.58</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="8">
         <v>1111.67</v>
       </c>
-      <c r="H57" s="8">
+      <c r="H57" s="7">
         <v>1093.75</v>
       </c>
-      <c r="I57" s="8">
+      <c r="I57" s="7">
         <v>1092.5</v>
       </c>
-      <c r="J57" s="8">
+      <c r="J57" s="7">
         <v>1093.33</v>
       </c>
-      <c r="K57" s="8">
+      <c r="K57" s="7">
         <v>1092.08</v>
       </c>
     </row>
@@ -3268,10 +3154,10 @@
       <c r="A58" s="5">
         <v>476.25</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58" s="7">
         <v>510</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C58" s="7">
         <v>527.5</v>
       </c>
       <c r="D58" s="5">
@@ -3283,19 +3169,19 @@
       <c r="F58" s="4">
         <v>552.08299999999997</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="8">
         <v>500.83300000000003</v>
       </c>
-      <c r="H58" s="8">
+      <c r="H58" s="7">
         <v>484.58300000000003</v>
       </c>
-      <c r="I58" s="8">
+      <c r="I58" s="7">
         <v>490.83300000000003</v>
       </c>
-      <c r="J58" s="8">
+      <c r="J58" s="7">
         <v>495.83300000000003</v>
       </c>
-      <c r="K58" s="8">
+      <c r="K58" s="7">
         <v>484.58300000000003</v>
       </c>
     </row>
@@ -3303,10 +3189,10 @@
       <c r="A59" s="5">
         <v>833.33299999999997</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="7">
         <v>835.83299999999997</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C59" s="7">
         <v>884.16700000000003</v>
       </c>
       <c r="D59" s="5">
@@ -3318,19 +3204,19 @@
       <c r="F59" s="4">
         <v>909.58299999999997</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="8">
         <v>852.91700000000003</v>
       </c>
-      <c r="H59" s="8">
+      <c r="H59" s="7">
         <v>790.41700000000003</v>
       </c>
-      <c r="I59" s="8">
+      <c r="I59" s="7">
         <v>773.75</v>
       </c>
-      <c r="J59" s="8">
+      <c r="J59" s="7">
         <v>852.91700000000003</v>
       </c>
-      <c r="K59" s="8">
+      <c r="K59" s="7">
         <v>827.5</v>
       </c>
     </row>
@@ -3338,10 +3224,10 @@
       <c r="A60" s="5">
         <v>640.83299999999997</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="7">
         <v>681.66700000000003</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C60" s="7">
         <v>720</v>
       </c>
       <c r="D60" s="5">
@@ -3353,19 +3239,19 @@
       <c r="F60" s="4">
         <v>670.41700000000003</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="8">
         <v>762.91700000000003</v>
       </c>
-      <c r="H60" s="8">
+      <c r="H60" s="7">
         <v>675.41700000000003</v>
       </c>
-      <c r="I60" s="8">
+      <c r="I60" s="7">
         <v>672.91700000000003</v>
       </c>
-      <c r="J60" s="8">
+      <c r="J60" s="7">
         <v>657.08299999999997</v>
       </c>
-      <c r="K60" s="8">
+      <c r="K60" s="7">
         <v>689.16700000000003</v>
       </c>
     </row>
@@ -3373,10 +3259,10 @@
       <c r="A61" s="5">
         <v>670.41700000000003</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61" s="7">
         <v>700.83299999999997</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C61" s="7">
         <v>692.91700000000003</v>
       </c>
       <c r="D61" s="5">
@@ -3388,19 +3274,19 @@
       <c r="F61" s="4">
         <v>724.58299999999997</v>
       </c>
-      <c r="G61" s="9">
+      <c r="G61" s="8">
         <v>701.66700000000003</v>
       </c>
-      <c r="H61" s="8">
+      <c r="H61" s="7">
         <v>682.08299999999997</v>
       </c>
-      <c r="I61" s="8">
+      <c r="I61" s="7">
         <v>670.41700000000003</v>
       </c>
-      <c r="J61" s="8">
+      <c r="J61" s="7">
         <v>673.75</v>
       </c>
-      <c r="K61" s="8">
+      <c r="K61" s="7">
         <v>675.83299999999997</v>
       </c>
     </row>
@@ -3408,10 +3294,10 @@
       <c r="A62" s="5">
         <v>361.25</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="7">
         <v>414.16699999999997</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C62" s="7">
         <v>436.25</v>
       </c>
       <c r="D62" s="5">
@@ -3423,19 +3309,19 @@
       <c r="F62" s="4">
         <v>471.25</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G62" s="8">
         <v>400.83300000000003</v>
       </c>
-      <c r="H62" s="8">
+      <c r="H62" s="7">
         <v>379.58300000000003</v>
       </c>
-      <c r="I62" s="8">
+      <c r="I62" s="7">
         <v>374.58300000000003</v>
       </c>
-      <c r="J62" s="8">
+      <c r="J62" s="7">
         <v>408.75</v>
       </c>
-      <c r="K62" s="8">
+      <c r="K62" s="7">
         <v>366.66699999999997</v>
       </c>
     </row>
@@ -3443,10 +3329,10 @@
       <c r="A63" s="5">
         <v>651.66700000000003</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B63" s="7">
         <v>643.33299999999997</v>
       </c>
-      <c r="C63" s="8">
+      <c r="C63" s="7">
         <v>594.58299999999997</v>
       </c>
       <c r="D63" s="5">
@@ -3458,19 +3344,19 @@
       <c r="F63" s="4">
         <v>600.83299999999997</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="8">
         <v>610.83299999999997</v>
       </c>
-      <c r="H63" s="8">
+      <c r="H63" s="7">
         <v>610</v>
       </c>
-      <c r="I63" s="8">
+      <c r="I63" s="7">
         <v>626.25</v>
       </c>
-      <c r="J63" s="8">
+      <c r="J63" s="7">
         <v>604.16700000000003</v>
       </c>
-      <c r="K63" s="8">
+      <c r="K63" s="7">
         <v>578.75</v>
       </c>
     </row>
@@ -3478,10 +3364,10 @@
       <c r="A64" s="5">
         <v>356.66699999999997</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64" s="7">
         <v>415</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C64" s="7">
         <v>417.91699999999997</v>
       </c>
       <c r="D64" s="5">
@@ -3493,19 +3379,19 @@
       <c r="F64" s="4">
         <v>427.5</v>
       </c>
-      <c r="G64" s="9">
+      <c r="G64" s="8">
         <v>430.83300000000003</v>
       </c>
-      <c r="H64" s="8">
+      <c r="H64" s="7">
         <v>382.5</v>
       </c>
-      <c r="I64" s="8">
+      <c r="I64" s="7">
         <v>359.58300000000003</v>
       </c>
-      <c r="J64" s="8">
+      <c r="J64" s="7">
         <v>380.83300000000003</v>
       </c>
-      <c r="K64" s="8">
+      <c r="K64" s="7">
         <v>405.41699999999997</v>
       </c>
     </row>
@@ -3513,10 +3399,10 @@
       <c r="A65" s="5">
         <v>715.83299999999997</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="7">
         <v>734.58299999999997</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C65" s="7">
         <v>703.75</v>
       </c>
       <c r="D65" s="5">
@@ -3528,19 +3414,19 @@
       <c r="F65" s="4">
         <v>714.16700000000003</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G65" s="8">
         <v>689.16700000000003</v>
       </c>
-      <c r="H65" s="8">
+      <c r="H65" s="7">
         <v>723.33299999999997</v>
       </c>
-      <c r="I65" s="8">
+      <c r="I65" s="7">
         <v>742.5</v>
       </c>
-      <c r="J65" s="8">
+      <c r="J65" s="7">
         <v>724.58299999999997</v>
       </c>
-      <c r="K65" s="8">
+      <c r="K65" s="7">
         <v>686.66700000000003</v>
       </c>
     </row>
@@ -3548,10 +3434,10 @@
       <c r="A66" s="5">
         <v>406.66699999999997</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="7">
         <v>412.91699999999997</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C66" s="7">
         <v>419.58300000000003</v>
       </c>
       <c r="D66" s="5">
@@ -3563,19 +3449,19 @@
       <c r="F66" s="4">
         <v>385.83300000000003</v>
       </c>
-      <c r="G66" s="9">
+      <c r="G66" s="8">
         <v>412.5</v>
       </c>
-      <c r="H66" s="8">
+      <c r="H66" s="7">
         <v>417.5</v>
       </c>
-      <c r="I66" s="8">
+      <c r="I66" s="7">
         <v>419.16699999999997</v>
       </c>
-      <c r="J66" s="8">
+      <c r="J66" s="7">
         <v>440.41699999999997</v>
       </c>
-      <c r="K66" s="8">
+      <c r="K66" s="7">
         <v>410.83300000000003</v>
       </c>
     </row>
@@ -3583,10 +3469,10 @@
       <c r="A67" s="5">
         <v>612.5</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B67" s="7">
         <v>574.16700000000003</v>
       </c>
-      <c r="C67" s="8">
+      <c r="C67" s="7">
         <v>554.58299999999997</v>
       </c>
       <c r="D67" s="5">
@@ -3598,19 +3484,19 @@
       <c r="F67" s="4">
         <v>589.16700000000003</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="8">
         <v>557.91700000000003</v>
       </c>
-      <c r="H67" s="8">
+      <c r="H67" s="7">
         <v>535.41700000000003</v>
       </c>
-      <c r="I67" s="8">
+      <c r="I67" s="7">
         <v>585</v>
       </c>
-      <c r="J67" s="8">
+      <c r="J67" s="7">
         <v>563.75</v>
       </c>
-      <c r="K67" s="8">
+      <c r="K67" s="7">
         <v>558.33299999999997</v>
       </c>
     </row>
@@ -3618,10 +3504,10 @@
       <c r="A68" s="5">
         <v>363.33300000000003</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B68" s="7">
         <v>431.66699999999997</v>
       </c>
-      <c r="C68" s="8">
+      <c r="C68" s="7">
         <v>360.41699999999997</v>
       </c>
       <c r="D68" s="5">
@@ -3633,19 +3519,19 @@
       <c r="F68" s="4">
         <v>380.83300000000003</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="8">
         <v>438.75</v>
       </c>
-      <c r="H68" s="8">
+      <c r="H68" s="7">
         <v>372.08300000000003</v>
       </c>
-      <c r="I68" s="8">
+      <c r="I68" s="7">
         <v>337.5</v>
       </c>
-      <c r="J68" s="8">
+      <c r="J68" s="7">
         <v>392.91699999999997</v>
       </c>
-      <c r="K68" s="8">
+      <c r="K68" s="7">
         <v>355.83300000000003</v>
       </c>
     </row>
@@ -3653,10 +3539,10 @@
       <c r="A69" s="5">
         <v>1292.92</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="7">
         <v>1387.92</v>
       </c>
-      <c r="C69" s="8">
+      <c r="C69" s="7">
         <v>1402.92</v>
       </c>
       <c r="D69" s="5">
@@ -3668,19 +3554,19 @@
       <c r="F69" s="4">
         <v>1429.58</v>
       </c>
-      <c r="G69" s="9">
+      <c r="G69" s="8">
         <v>1377.92</v>
       </c>
-      <c r="H69" s="8">
+      <c r="H69" s="7">
         <v>1322.5</v>
       </c>
-      <c r="I69" s="8">
+      <c r="I69" s="7">
         <v>1297.92</v>
       </c>
-      <c r="J69" s="8">
+      <c r="J69" s="7">
         <v>1317.08</v>
       </c>
-      <c r="K69" s="8">
+      <c r="K69" s="7">
         <v>1312.92</v>
       </c>
     </row>
@@ -3688,10 +3574,10 @@
       <c r="A70" s="5">
         <v>1101.25</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B70" s="7">
         <v>1180.42</v>
       </c>
-      <c r="C70" s="8">
+      <c r="C70" s="7">
         <v>1072.92</v>
       </c>
       <c r="D70" s="5">
@@ -3703,19 +3589,19 @@
       <c r="F70" s="4">
         <v>1173.75</v>
       </c>
-      <c r="G70" s="9">
+      <c r="G70" s="8">
         <v>1125.42</v>
       </c>
-      <c r="H70" s="8">
+      <c r="H70" s="7">
         <v>1141.67</v>
       </c>
-      <c r="I70" s="8">
+      <c r="I70" s="7">
         <v>1127.08</v>
       </c>
-      <c r="J70" s="8">
+      <c r="J70" s="7">
         <v>1109.58</v>
       </c>
-      <c r="K70" s="8">
+      <c r="K70" s="7">
         <v>1158.75</v>
       </c>
     </row>
@@ -3723,10 +3609,10 @@
       <c r="A71" s="5">
         <v>1048.33</v>
       </c>
-      <c r="B71" s="8">
+      <c r="B71" s="7">
         <v>1040.42</v>
       </c>
-      <c r="C71" s="8">
+      <c r="C71" s="7">
         <v>1064.58</v>
       </c>
       <c r="D71" s="5">
@@ -3738,19 +3624,19 @@
       <c r="F71" s="4">
         <v>1026.67</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="8">
         <v>1027.08</v>
       </c>
-      <c r="H71" s="8">
+      <c r="H71" s="7">
         <v>970.83299999999997</v>
       </c>
-      <c r="I71" s="8">
+      <c r="I71" s="7">
         <v>1045</v>
       </c>
-      <c r="J71" s="8">
+      <c r="J71" s="7">
         <v>997.08299999999997</v>
       </c>
-      <c r="K71" s="8">
+      <c r="K71" s="7">
         <v>1036.67</v>
       </c>
     </row>
@@ -3758,10 +3644,10 @@
       <c r="A72" s="5">
         <v>780</v>
       </c>
-      <c r="B72" s="8">
+      <c r="B72" s="7">
         <v>797.08299999999997</v>
       </c>
-      <c r="C72" s="8">
+      <c r="C72" s="7">
         <v>808.75</v>
       </c>
       <c r="D72" s="5">
@@ -3773,19 +3659,19 @@
       <c r="F72" s="4">
         <v>785.83299999999997</v>
       </c>
-      <c r="G72" s="9">
+      <c r="G72" s="8">
         <v>753.75</v>
       </c>
-      <c r="H72" s="8">
+      <c r="H72" s="7">
         <v>720</v>
       </c>
-      <c r="I72" s="8">
+      <c r="I72" s="7">
         <v>741.66700000000003</v>
       </c>
-      <c r="J72" s="8">
+      <c r="J72" s="7">
         <v>777.08299999999997</v>
       </c>
-      <c r="K72" s="8">
+      <c r="K72" s="7">
         <v>748.33299999999997</v>
       </c>
     </row>
@@ -3793,10 +3679,10 @@
       <c r="A73" s="5">
         <v>1170</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B73" s="7">
         <v>1225.83</v>
       </c>
-      <c r="C73" s="8">
+      <c r="C73" s="7">
         <v>1215</v>
       </c>
       <c r="D73" s="5">
@@ -3808,19 +3694,19 @@
       <c r="F73" s="4">
         <v>1256.25</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="8">
         <v>1202.5</v>
       </c>
-      <c r="H73" s="8">
+      <c r="H73" s="7">
         <v>1173.75</v>
       </c>
-      <c r="I73" s="8">
+      <c r="I73" s="7">
         <v>1148.75</v>
       </c>
-      <c r="J73" s="8">
+      <c r="J73" s="7">
         <v>1150.42</v>
       </c>
-      <c r="K73" s="8">
+      <c r="K73" s="7">
         <v>1172.92</v>
       </c>
     </row>
@@ -3828,10 +3714,10 @@
       <c r="A74" s="5">
         <v>883.33299999999997</v>
       </c>
-      <c r="B74" s="8">
+      <c r="B74" s="7">
         <v>831.66700000000003</v>
       </c>
-      <c r="C74" s="8">
+      <c r="C74" s="7">
         <v>879.16700000000003</v>
       </c>
       <c r="D74" s="5">
@@ -3843,19 +3729,19 @@
       <c r="F74" s="4">
         <v>887.91700000000003</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="8">
         <v>858.33299999999997</v>
       </c>
-      <c r="H74" s="8">
+      <c r="H74" s="7">
         <v>824.58299999999997</v>
       </c>
-      <c r="I74" s="8">
+      <c r="I74" s="7">
         <v>818.75</v>
       </c>
-      <c r="J74" s="8">
+      <c r="J74" s="7">
         <v>824.58299999999997</v>
       </c>
-      <c r="K74" s="8">
+      <c r="K74" s="7">
         <v>854.58299999999997</v>
       </c>
     </row>
@@ -3863,10 +3749,10 @@
       <c r="A75" s="5">
         <v>583.75</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B75" s="7">
         <v>615</v>
       </c>
-      <c r="C75" s="8">
+      <c r="C75" s="7">
         <v>562.91700000000003</v>
       </c>
       <c r="D75" s="5">
@@ -3878,19 +3764,19 @@
       <c r="F75" s="4">
         <v>647.5</v>
       </c>
-      <c r="G75" s="9">
+      <c r="G75" s="8">
         <v>567.08299999999997</v>
       </c>
-      <c r="H75" s="8">
+      <c r="H75" s="7">
         <v>622.5</v>
       </c>
-      <c r="I75" s="8">
+      <c r="I75" s="7">
         <v>582.5</v>
       </c>
-      <c r="J75" s="8">
+      <c r="J75" s="7">
         <v>589.16700000000003</v>
       </c>
-      <c r="K75" s="8">
+      <c r="K75" s="7">
         <v>552.08299999999997</v>
       </c>
     </row>
@@ -3898,10 +3784,10 @@
       <c r="A76" s="5">
         <v>542.91700000000003</v>
       </c>
-      <c r="B76" s="8">
+      <c r="B76" s="7">
         <v>502.5</v>
       </c>
-      <c r="C76" s="8">
+      <c r="C76" s="7">
         <v>522.08299999999997</v>
       </c>
       <c r="D76" s="5">
@@ -3913,19 +3799,19 @@
       <c r="F76" s="4">
         <v>570</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G76" s="8">
         <v>529.58299999999997</v>
       </c>
-      <c r="H76" s="8">
+      <c r="H76" s="7">
         <v>491.66699999999997</v>
       </c>
-      <c r="I76" s="8">
+      <c r="I76" s="7">
         <v>537.5</v>
       </c>
-      <c r="J76" s="8">
+      <c r="J76" s="7">
         <v>485</v>
       </c>
-      <c r="K76" s="8">
+      <c r="K76" s="7">
         <v>522.08299999999997</v>
       </c>
     </row>
@@ -3933,10 +3819,10 @@
       <c r="A77" s="5">
         <v>932.08299999999997</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="7">
         <v>1027.08</v>
       </c>
-      <c r="C77" s="8">
+      <c r="C77" s="7">
         <v>1018.33</v>
       </c>
       <c r="D77" s="5">
@@ -3948,19 +3834,19 @@
       <c r="F77" s="4">
         <v>1008.75</v>
       </c>
-      <c r="G77" s="9">
+      <c r="G77" s="8">
         <v>1000</v>
       </c>
-      <c r="H77" s="8">
+      <c r="H77" s="7">
         <v>924.16700000000003</v>
       </c>
-      <c r="I77" s="8">
+      <c r="I77" s="7">
         <v>815.83299999999997</v>
       </c>
-      <c r="J77" s="8">
+      <c r="J77" s="7">
         <v>930.83299999999997</v>
       </c>
-      <c r="K77" s="8">
+      <c r="K77" s="7">
         <v>926.25</v>
       </c>
     </row>
@@ -3968,10 +3854,10 @@
       <c r="A78" s="5">
         <v>685.41700000000003</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B78" s="7">
         <v>717.91700000000003</v>
       </c>
-      <c r="C78" s="8">
+      <c r="C78" s="7">
         <v>686.66700000000003</v>
       </c>
       <c r="D78" s="5">
@@ -3983,19 +3869,19 @@
       <c r="F78" s="4">
         <v>742.91700000000003</v>
       </c>
-      <c r="G78" s="9">
+      <c r="G78" s="8">
         <v>710.83299999999997</v>
       </c>
-      <c r="H78" s="8">
+      <c r="H78" s="7">
         <v>705</v>
       </c>
-      <c r="I78" s="8">
+      <c r="I78" s="7">
         <v>650.83299999999997</v>
       </c>
-      <c r="J78" s="8">
+      <c r="J78" s="7">
         <v>686.66700000000003</v>
       </c>
-      <c r="K78" s="8">
+      <c r="K78" s="7">
         <v>678.75</v>
       </c>
     </row>
@@ -4003,10 +3889,10 @@
       <c r="A79" s="5">
         <v>868.33299999999997</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="7">
         <v>910</v>
       </c>
-      <c r="C79" s="8">
+      <c r="C79" s="7">
         <v>933.75</v>
       </c>
       <c r="D79" s="5">
@@ -4018,19 +3904,19 @@
       <c r="F79" s="4">
         <v>978.75</v>
       </c>
-      <c r="G79" s="9">
+      <c r="G79" s="8">
         <v>915</v>
       </c>
-      <c r="H79" s="8">
+      <c r="H79" s="7">
         <v>916.25</v>
       </c>
-      <c r="I79" s="8">
+      <c r="I79" s="7">
         <v>927.91700000000003</v>
       </c>
-      <c r="J79" s="8">
+      <c r="J79" s="7">
         <v>847.08299999999997</v>
       </c>
-      <c r="K79" s="8">
+      <c r="K79" s="7">
         <v>847.5</v>
       </c>
     </row>
@@ -4038,10 +3924,10 @@
       <c r="A80" s="5">
         <v>799.16700000000003</v>
       </c>
-      <c r="B80" s="8">
+      <c r="B80" s="7">
         <v>815</v>
       </c>
-      <c r="C80" s="8">
+      <c r="C80" s="7">
         <v>732.08299999999997</v>
       </c>
       <c r="D80" s="5">
@@ -4053,19 +3939,19 @@
       <c r="F80" s="4">
         <v>812.08299999999997</v>
       </c>
-      <c r="G80" s="9">
+      <c r="G80" s="8">
         <v>850.83299999999997</v>
       </c>
-      <c r="H80" s="8">
+      <c r="H80" s="7">
         <v>819.58299999999997</v>
       </c>
-      <c r="I80" s="8">
+      <c r="I80" s="7">
         <v>853.75</v>
       </c>
-      <c r="J80" s="8">
+      <c r="J80" s="7">
         <v>840.41700000000003</v>
       </c>
-      <c r="K80" s="8">
+      <c r="K80" s="7">
         <v>818.33299999999997</v>
       </c>
     </row>
@@ -4073,10 +3959,10 @@
       <c r="A81" s="5">
         <v>1159.58</v>
       </c>
-      <c r="B81" s="8">
+      <c r="B81" s="7">
         <v>1211.67</v>
       </c>
-      <c r="C81" s="8">
+      <c r="C81" s="7">
         <v>1195</v>
       </c>
       <c r="D81" s="5">
@@ -4088,19 +3974,19 @@
       <c r="F81" s="4">
         <v>1315</v>
       </c>
-      <c r="G81" s="9">
+      <c r="G81" s="8">
         <v>1192.92</v>
       </c>
-      <c r="H81" s="8">
+      <c r="H81" s="7">
         <v>1181.67</v>
       </c>
-      <c r="I81" s="8">
+      <c r="I81" s="7">
         <v>1144.58</v>
       </c>
-      <c r="J81" s="8">
+      <c r="J81" s="7">
         <v>1157.92</v>
       </c>
-      <c r="K81" s="8">
+      <c r="K81" s="7">
         <v>1157.5</v>
       </c>
     </row>
@@ -4108,10 +3994,10 @@
       <c r="A82" s="5">
         <v>969.58299999999997</v>
       </c>
-      <c r="B82" s="8">
+      <c r="B82" s="7">
         <v>1000</v>
       </c>
-      <c r="C82" s="8">
+      <c r="C82" s="7">
         <v>962.5</v>
       </c>
       <c r="D82" s="5">
@@ -4123,19 +4009,19 @@
       <c r="F82" s="4">
         <v>991.66700000000003</v>
       </c>
-      <c r="G82" s="9">
+      <c r="G82" s="8">
         <v>947.91700000000003</v>
       </c>
-      <c r="H82" s="8">
+      <c r="H82" s="7">
         <v>932.5</v>
       </c>
-      <c r="I82" s="8">
+      <c r="I82" s="7">
         <v>932.91700000000003</v>
       </c>
-      <c r="J82" s="8">
+      <c r="J82" s="7">
         <v>921.25</v>
       </c>
-      <c r="K82" s="8">
+      <c r="K82" s="7">
         <v>965.83299999999997</v>
       </c>
     </row>
@@ -4143,10 +4029,10 @@
       <c r="A83" s="5">
         <v>727.08299999999997</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B83" s="7">
         <v>852.91700000000003</v>
       </c>
-      <c r="C83" s="8">
+      <c r="C83" s="7">
         <v>780</v>
       </c>
       <c r="D83" s="5">
@@ -4158,19 +4044,19 @@
       <c r="F83" s="4">
         <v>778.75</v>
       </c>
-      <c r="G83" s="9">
+      <c r="G83" s="8">
         <v>755</v>
       </c>
-      <c r="H83" s="8">
+      <c r="H83" s="7">
         <v>747.91700000000003</v>
       </c>
-      <c r="I83" s="8">
+      <c r="I83" s="7">
         <v>761.25</v>
       </c>
-      <c r="J83" s="8">
+      <c r="J83" s="7">
         <v>773.75</v>
       </c>
-      <c r="K83" s="8">
+      <c r="K83" s="7">
         <v>770.41700000000003</v>
       </c>
     </row>
@@ -4178,10 +4064,10 @@
       <c r="A84" s="5">
         <v>387.08300000000003</v>
       </c>
-      <c r="B84" s="8">
+      <c r="B84" s="7">
         <v>377.91699999999997</v>
       </c>
-      <c r="C84" s="8">
+      <c r="C84" s="7">
         <v>307.5</v>
       </c>
       <c r="D84" s="5">
@@ -4193,19 +4079,19 @@
       <c r="F84" s="4">
         <v>392.08300000000003</v>
       </c>
-      <c r="G84" s="9">
+      <c r="G84" s="8">
         <v>326.66699999999997</v>
       </c>
-      <c r="H84" s="8">
+      <c r="H84" s="7">
         <v>352.91699999999997</v>
       </c>
-      <c r="I84" s="8">
+      <c r="I84" s="7">
         <v>422.91699999999997</v>
       </c>
-      <c r="J84" s="8">
+      <c r="J84" s="7">
         <v>416.25</v>
       </c>
-      <c r="K84" s="8">
+      <c r="K84" s="7">
         <v>330.41699999999997</v>
       </c>
     </row>
@@ -4213,10 +4099,10 @@
       <c r="A85" s="5">
         <v>1499.58</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B85" s="7">
         <v>1575</v>
       </c>
-      <c r="C85" s="8">
+      <c r="C85" s="7">
         <v>1549.58</v>
       </c>
       <c r="D85" s="5">
@@ -4228,19 +4114,19 @@
       <c r="F85" s="4">
         <v>1593.33</v>
       </c>
-      <c r="G85" s="9">
+      <c r="G85" s="8">
         <v>1563.33</v>
       </c>
-      <c r="H85" s="8">
+      <c r="H85" s="7">
         <v>1539.58</v>
       </c>
-      <c r="I85" s="8">
+      <c r="I85" s="7">
         <v>1505.83</v>
       </c>
-      <c r="J85" s="8">
+      <c r="J85" s="7">
         <v>1493.33</v>
       </c>
-      <c r="K85" s="8">
+      <c r="K85" s="7">
         <v>1515</v>
       </c>
     </row>
@@ -4248,10 +4134,10 @@
       <c r="A86" s="5">
         <v>819.58299999999997</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="7">
         <v>830</v>
       </c>
-      <c r="C86" s="8">
+      <c r="C86" s="7">
         <v>841.25</v>
       </c>
       <c r="D86" s="5">
@@ -4263,19 +4149,19 @@
       <c r="F86" s="4">
         <v>861.66700000000003</v>
       </c>
-      <c r="G86" s="9">
+      <c r="G86" s="8">
         <v>870</v>
       </c>
-      <c r="H86" s="8">
+      <c r="H86" s="7">
         <v>864.58299999999997</v>
       </c>
-      <c r="I86" s="8">
+      <c r="I86" s="7">
         <v>824.16700000000003</v>
       </c>
-      <c r="J86" s="8">
+      <c r="J86" s="7">
         <v>863.33299999999997</v>
       </c>
-      <c r="K86" s="8">
+      <c r="K86" s="7">
         <v>871.66700000000003</v>
       </c>
     </row>
@@ -4283,10 +4169,10 @@
       <c r="A87" s="5">
         <v>445</v>
       </c>
-      <c r="B87" s="8">
+      <c r="B87" s="7">
         <v>399.16699999999997</v>
       </c>
-      <c r="C87" s="8">
+      <c r="C87" s="7">
         <v>362.5</v>
       </c>
       <c r="D87" s="5">
@@ -4298,19 +4184,19 @@
       <c r="F87" s="4">
         <v>372.5</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="8">
         <v>402.5</v>
       </c>
-      <c r="H87" s="8">
+      <c r="H87" s="7">
         <v>425.41699999999997</v>
       </c>
-      <c r="I87" s="8">
+      <c r="I87" s="7">
         <v>411.66699999999997</v>
       </c>
-      <c r="J87" s="8">
+      <c r="J87" s="7">
         <v>412.91699999999997</v>
       </c>
-      <c r="K87" s="8">
+      <c r="K87" s="7">
         <v>419.16699999999997</v>
       </c>
     </row>
@@ -4318,10 +4204,10 @@
       <c r="A88" s="5">
         <v>430.83300000000003</v>
       </c>
-      <c r="B88" s="8">
+      <c r="B88" s="7">
         <v>357.5</v>
       </c>
-      <c r="C88" s="8">
+      <c r="C88" s="7">
         <v>418.33300000000003</v>
       </c>
       <c r="D88" s="5">
@@ -4333,19 +4219,19 @@
       <c r="F88" s="4">
         <v>317.5</v>
       </c>
-      <c r="G88" s="9">
+      <c r="G88" s="8">
         <v>350</v>
       </c>
-      <c r="H88" s="8">
+      <c r="H88" s="7">
         <v>449.58300000000003</v>
       </c>
-      <c r="I88" s="8">
+      <c r="I88" s="7">
         <v>411.66699999999997</v>
       </c>
-      <c r="J88" s="8">
+      <c r="J88" s="7">
         <v>402.91699999999997</v>
       </c>
-      <c r="K88" s="8">
+      <c r="K88" s="7">
         <v>362.5</v>
       </c>
     </row>
@@ -4356,30 +4242,30 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A89:Z128 B4:Z88">
-    <cfRule type="expression" dxfId="11" priority="50">
+    <cfRule type="expression" dxfId="7" priority="50">
       <formula>A4=SMALL($A4:$Z4,1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="51">
+    <cfRule type="expression" dxfId="6" priority="51">
       <formula>A4=SMALL($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="52">
+    <cfRule type="expression" dxfId="5" priority="52">
       <formula>A4=LARGE($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="53">
+    <cfRule type="expression" dxfId="4" priority="53">
       <formula>A4=LARGE($A4:$Z4,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A88">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>A4=SMALL($A4:$Z4,1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>A4=SMALL($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>A4=LARGE($A4:$Z4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>A4=LARGE($A4:$Z4,1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update perturb strategy. bug fix on repair(). log stash. remove raw log.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/compare--20150501--GreedyInit+Tabu.xlsx
+++ b/INRC2_Simulator/log/compare--20150501--GreedyInit+Tabu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="19170" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -88,11 +88,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;1.2,1.2</t>
+    <t>2;1.2,1.2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>2;1.2,1.2</t>
+    <t>1;0.8,0.8</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1149,7 +1149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1166,10 +1168,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>

</xml_diff>